<commit_message>
fix none description err
</commit_message>
<xml_diff>
--- a/src/tests/excel/测试和示例表.xlsx
+++ b/src/tests/excel/测试和示例表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\stanley\zes-excel-exporter\src\tests\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6499C312-9316-4C3C-9C59-3CA45D84B026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBFF581-DBD9-4387-82E9-D172C8ACB57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="测试数据1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="134">
   <si>
     <t>testdata1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -493,6 +493,10 @@
   </si>
   <si>
     <t>ID#c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tttt</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -928,13 +932,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K3" sqref="K3"/>
+      <selection pane="bottomRight" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -946,13 +950,13 @@
     <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -996,7 +1000,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1039,8 +1043,11 @@
       <c r="N3" s="8" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O3" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1001</v>
       </c>
@@ -1084,7 +1091,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1002</v>
       </c>
@@ -1128,7 +1135,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1003</v>
       </c>
@@ -1172,7 +1179,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>119</v>
       </c>
@@ -1216,7 +1223,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1005</v>
       </c>
@@ -1260,7 +1267,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1006</v>
       </c>
@@ -1304,7 +1311,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>1007</v>
       </c>
@@ -1348,7 +1355,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>1008</v>
       </c>
@@ -1392,7 +1399,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>1009</v>
       </c>
@@ -1436,7 +1443,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>1010</v>
       </c>
@@ -1480,7 +1487,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>1011</v>
       </c>
@@ -1524,7 +1531,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>1012</v>
       </c>
@@ -1568,7 +1575,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>124</v>
       </c>
@@ -4791,7 +4798,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283D2224-75B9-48C8-B672-2B433B31B801}">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ignore line start with *
</commit_message>
<xml_diff>
--- a/src/tests/excel/测试和示例表.xlsx
+++ b/src/tests/excel/测试和示例表.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\stanley\zes-excel-exporter\src\tests\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBFF581-DBD9-4387-82E9-D172C8ACB57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F7C717-8173-48F5-8CBE-1F8AF60F75F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="测试数据1" sheetId="1" r:id="rId1"/>
@@ -320,10 +320,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ID, s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>clientdata</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -497,6 +493,10 @@
   </si>
   <si>
     <t>tttt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID#s</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -938,7 +938,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O4" sqref="O4"/>
+      <selection pane="bottomRight" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -946,7 +946,9 @@
     <col min="1" max="1" width="26.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="60.375" style="1" customWidth="1"/>
     <col min="3" max="4" width="17.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="14" width="16.25" style="1" customWidth="1"/>
+    <col min="5" max="9" width="16.25" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5" style="1" customWidth="1"/>
+    <col min="11" max="14" width="16.25" style="1" customWidth="1"/>
     <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -961,19 +963,19 @@
         <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>96</v>
-      </c>
       <c r="F2" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>4</v>
@@ -985,19 +987,19 @@
         <v>6</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1005,19 +1007,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>14</v>
@@ -1032,19 +1034,19 @@
         <v>17</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>18</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -1052,7 +1054,7 @@
         <v>1001</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -1096,7 +1098,7 @@
         <v>1002</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
@@ -1140,7 +1142,7 @@
         <v>1003</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C6" s="1">
         <v>3</v>
@@ -1181,10 +1183,10 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C7" s="1">
         <v>4</v>
@@ -1228,7 +1230,7 @@
         <v>1005</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C8" s="1">
         <v>5</v>
@@ -1272,7 +1274,7 @@
         <v>1006</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C9" s="1">
         <v>6</v>
@@ -1316,7 +1318,7 @@
         <v>1007</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C10" s="1">
         <v>7</v>
@@ -1360,7 +1362,7 @@
         <v>1008</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C11" s="1">
         <v>8</v>
@@ -1404,7 +1406,7 @@
         <v>1009</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C12" s="1">
         <v>9</v>
@@ -1448,7 +1450,7 @@
         <v>1010</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C13" s="1">
         <v>10</v>
@@ -1492,7 +1494,7 @@
         <v>1011</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C14" s="1">
         <v>11</v>
@@ -1536,7 +1538,7 @@
         <v>1012</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C15" s="1">
         <v>12</v>
@@ -1577,10 +1579,10 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C16" s="1">
         <v>13</v>
@@ -1624,7 +1626,7 @@
         <v>1014</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C17" s="1">
         <v>14</v>
@@ -1668,7 +1670,7 @@
         <v>1015</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C18" s="1">
         <v>15</v>
@@ -1712,7 +1714,7 @@
         <v>1016</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C19" s="1">
         <v>16</v>
@@ -1756,7 +1758,7 @@
         <v>1017</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C20" s="1">
         <v>17</v>
@@ -1800,7 +1802,7 @@
         <v>1018</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C21" s="1">
         <v>18</v>
@@ -1844,7 +1846,7 @@
         <v>1019</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C22" s="1">
         <v>19</v>
@@ -1888,7 +1890,7 @@
         <v>1020</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C23" s="1">
         <v>20</v>
@@ -1932,7 +1934,7 @@
         <v>1021</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C24" s="1">
         <v>21</v>
@@ -1976,7 +1978,7 @@
         <v>1022</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C25" s="1">
         <v>22</v>
@@ -2020,7 +2022,7 @@
         <v>1023</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C26" s="1">
         <v>23</v>
@@ -2064,7 +2066,7 @@
         <v>1024</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C27" s="1">
         <v>24</v>
@@ -2108,7 +2110,7 @@
         <v>1025</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C28" s="1">
         <v>25</v>
@@ -2152,7 +2154,7 @@
         <v>1026</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C29" s="1">
         <v>26</v>
@@ -2196,7 +2198,7 @@
         <v>1027</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C30" s="1">
         <v>27</v>
@@ -2240,7 +2242,7 @@
         <v>1028</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C31" s="1">
         <v>28</v>
@@ -2284,7 +2286,7 @@
         <v>1029</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C32" s="1">
         <v>29</v>
@@ -2328,7 +2330,7 @@
         <v>1030</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C33" s="1">
         <v>30</v>
@@ -2372,7 +2374,7 @@
         <v>1031</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C34" s="1">
         <v>31</v>
@@ -2416,7 +2418,7 @@
         <v>1032</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C35" s="1">
         <v>32</v>
@@ -2489,13 +2491,13 @@
         <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>4</v>
@@ -2507,16 +2509,16 @@
         <v>6</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -2524,7 +2526,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>12</v>
@@ -2548,10 +2550,10 @@
         <v>18</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -2559,7 +2561,7 @@
         <v>1001</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -2594,7 +2596,7 @@
         <v>1002</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
@@ -2629,7 +2631,7 @@
         <v>1003</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C6" s="1">
         <v>3</v>
@@ -2664,7 +2666,7 @@
         <v>1004</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C7" s="1">
         <v>4</v>
@@ -2699,7 +2701,7 @@
         <v>1005</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C8" s="1">
         <v>5</v>
@@ -2734,7 +2736,7 @@
         <v>1006</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C9" s="1">
         <v>6</v>
@@ -2769,7 +2771,7 @@
         <v>1007</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C10" s="1">
         <v>7</v>
@@ -2804,7 +2806,7 @@
         <v>1008</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C11" s="1">
         <v>8</v>
@@ -2839,7 +2841,7 @@
         <v>1009</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C12" s="1">
         <v>9</v>
@@ -2874,7 +2876,7 @@
         <v>1010</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C13" s="1">
         <v>10</v>
@@ -2909,7 +2911,7 @@
         <v>1011</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C14" s="1">
         <v>11</v>
@@ -2944,7 +2946,7 @@
         <v>1012</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C15" s="1">
         <v>12</v>
@@ -2979,7 +2981,7 @@
         <v>1013</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C16" s="1">
         <v>13</v>
@@ -3014,7 +3016,7 @@
         <v>1014</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C17" s="1">
         <v>14</v>
@@ -3049,7 +3051,7 @@
         <v>1015</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C18" s="1">
         <v>15</v>
@@ -3084,7 +3086,7 @@
         <v>1016</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C19" s="1">
         <v>16</v>
@@ -3119,7 +3121,7 @@
         <v>1017</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C20" s="1">
         <v>17</v>
@@ -3154,7 +3156,7 @@
         <v>1018</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C21" s="1">
         <v>18</v>
@@ -3189,7 +3191,7 @@
         <v>1019</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C22" s="1">
         <v>19</v>
@@ -3224,7 +3226,7 @@
         <v>1020</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C23" s="1">
         <v>20</v>
@@ -3259,7 +3261,7 @@
         <v>1021</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C24" s="1">
         <v>21</v>
@@ -3294,7 +3296,7 @@
         <v>1022</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C25" s="1">
         <v>22</v>
@@ -3329,7 +3331,7 @@
         <v>1023</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C26" s="1">
         <v>23</v>
@@ -3364,7 +3366,7 @@
         <v>1024</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C27" s="1">
         <v>24</v>
@@ -3399,7 +3401,7 @@
         <v>1025</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C28" s="1">
         <v>25</v>
@@ -3434,7 +3436,7 @@
         <v>1026</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C29" s="1">
         <v>26</v>
@@ -3469,7 +3471,7 @@
         <v>1027</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C30" s="1">
         <v>27</v>
@@ -3504,7 +3506,7 @@
         <v>1028</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C31" s="1">
         <v>28</v>
@@ -3539,7 +3541,7 @@
         <v>1029</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C32" s="1">
         <v>29</v>
@@ -3574,7 +3576,7 @@
         <v>1030</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C33" s="1">
         <v>30</v>
@@ -3609,7 +3611,7 @@
         <v>1031</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C34" s="1">
         <v>31</v>
@@ -3644,7 +3646,7 @@
         <v>1032</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C35" s="1">
         <v>32</v>
@@ -3685,7 +3687,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3702,7 +3704,7 @@
     </row>
     <row r="2" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>89</v>
+        <v>133</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>2</v>
@@ -4811,12 +4813,12 @@
   <sheetData>
     <row r="1" spans="1:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>2</v>
@@ -5925,12 +5927,12 @@
   <sheetData>
     <row r="1" spans="1:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>2</v>

</xml_diff>